<commit_message>
update stop at a point
</commit_message>
<xml_diff>
--- a/BACKUP/FRT.CAL.xlsx
+++ b/BACKUP/FRT.CAL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="159">
   <si>
     <t>VCH.NO</t>
   </si>
@@ -73,6 +73,12 @@
     <t>CREATED : 11/04/2021 23:05:55</t>
   </si>
   <si>
+    <t>CREATED : 11/04/2021 23:07:42</t>
+  </si>
+  <si>
+    <t>CREATED : 12/04/2021 09:43:37</t>
+  </si>
+  <si>
     <t>22591/RH/GKF/2021-22\902021/0</t>
   </si>
   <si>
@@ -427,10 +433,10 @@
     <t>RAMU WALA</t>
   </si>
   <si>
+    <t>JHUMBA</t>
+  </si>
+  <si>
     <t>nan</t>
-  </si>
-  <si>
-    <t>JHUMBA</t>
   </si>
   <si>
     <t>340</t>
@@ -842,7 +848,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -903,37 +909,37 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -947,37 +953,37 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="M3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -991,37 +997,37 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="M4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1035,37 +1041,37 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1079,37 +1085,37 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="M6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1123,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="N7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1167,37 +1173,37 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1211,37 +1217,37 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1255,37 +1261,37 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1299,37 +1305,37 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M11" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N11" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1343,37 +1349,37 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="M12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N12" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1387,37 +1393,37 @@
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1431,37 +1437,34 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="M14" t="s">
-        <v>139</v>
-      </c>
-      <c r="N14" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1475,37 +1478,34 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="L15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="M15" t="s">
-        <v>140</v>
-      </c>
-      <c r="N15" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1519,37 +1519,37 @@
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K16" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M16" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1563,37 +1563,37 @@
         <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K17" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L17" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M17" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N17" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1607,37 +1607,31 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K18" t="s">
-        <v>124</v>
-      </c>
-      <c r="L18" t="s">
-        <v>137</v>
-      </c>
-      <c r="M18" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="N18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1651,37 +1645,37 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K19" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1694,10 +1688,10 @@
         <v>18</v>
       </c>
       <c r="J21" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1707,6 +1701,1630 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" t="s">
+        <v>93</v>
+      </c>
+      <c r="J24" t="s">
+        <v>103</v>
+      </c>
+      <c r="K24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L24" t="s">
+        <v>129</v>
+      </c>
+      <c r="M24" t="s">
+        <v>141</v>
+      </c>
+      <c r="N24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" t="s">
+        <v>113</v>
+      </c>
+      <c r="L25" t="s">
+        <v>130</v>
+      </c>
+      <c r="M25" t="s">
+        <v>141</v>
+      </c>
+      <c r="N25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" t="s">
+        <v>105</v>
+      </c>
+      <c r="K26" t="s">
+        <v>114</v>
+      </c>
+      <c r="L26" t="s">
+        <v>131</v>
+      </c>
+      <c r="M26" t="s">
+        <v>141</v>
+      </c>
+      <c r="N26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" t="s">
+        <v>79</v>
+      </c>
+      <c r="I27" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" t="s">
+        <v>106</v>
+      </c>
+      <c r="K27" t="s">
+        <v>115</v>
+      </c>
+      <c r="L27" t="s">
+        <v>132</v>
+      </c>
+      <c r="M27" t="s">
+        <v>141</v>
+      </c>
+      <c r="N27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I28" t="s">
+        <v>97</v>
+      </c>
+      <c r="J28" t="s">
+        <v>107</v>
+      </c>
+      <c r="K28" t="s">
+        <v>116</v>
+      </c>
+      <c r="L28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M28" t="s">
+        <v>141</v>
+      </c>
+      <c r="N28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" t="s">
+        <v>97</v>
+      </c>
+      <c r="J29" t="s">
+        <v>107</v>
+      </c>
+      <c r="K29" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" t="s">
+        <v>134</v>
+      </c>
+      <c r="M29" t="s">
+        <v>142</v>
+      </c>
+      <c r="N29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I30" t="s">
+        <v>98</v>
+      </c>
+      <c r="J30" t="s">
+        <v>108</v>
+      </c>
+      <c r="K30" t="s">
+        <v>118</v>
+      </c>
+      <c r="L30" t="s">
+        <v>135</v>
+      </c>
+      <c r="M30" t="s">
+        <v>143</v>
+      </c>
+      <c r="N30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" t="s">
+        <v>99</v>
+      </c>
+      <c r="J31" t="s">
+        <v>109</v>
+      </c>
+      <c r="K31" t="s">
+        <v>119</v>
+      </c>
+      <c r="L31" t="s">
+        <v>136</v>
+      </c>
+      <c r="M31" t="s">
+        <v>143</v>
+      </c>
+      <c r="N31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" t="s">
+        <v>100</v>
+      </c>
+      <c r="J32" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" t="s">
+        <v>120</v>
+      </c>
+      <c r="L32" t="s">
+        <v>137</v>
+      </c>
+      <c r="M32" t="s">
+        <v>143</v>
+      </c>
+      <c r="N32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" t="s">
+        <v>85</v>
+      </c>
+      <c r="I33" t="s">
+        <v>101</v>
+      </c>
+      <c r="J33" t="s">
+        <v>110</v>
+      </c>
+      <c r="K33" t="s">
+        <v>121</v>
+      </c>
+      <c r="L33" t="s">
+        <v>134</v>
+      </c>
+      <c r="M33" t="s">
+        <v>141</v>
+      </c>
+      <c r="N33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" t="s">
+        <v>96</v>
+      </c>
+      <c r="J34" t="s">
+        <v>106</v>
+      </c>
+      <c r="K34" t="s">
+        <v>114</v>
+      </c>
+      <c r="L34" t="s">
+        <v>131</v>
+      </c>
+      <c r="M34" t="s">
+        <v>141</v>
+      </c>
+      <c r="N34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" t="s">
+        <v>70</v>
+      </c>
+      <c r="H35" t="s">
+        <v>87</v>
+      </c>
+      <c r="I35" t="s">
+        <v>96</v>
+      </c>
+      <c r="J35" t="s">
+        <v>106</v>
+      </c>
+      <c r="K35" t="s">
+        <v>121</v>
+      </c>
+      <c r="L35" t="s">
+        <v>134</v>
+      </c>
+      <c r="M35" t="s">
+        <v>141</v>
+      </c>
+      <c r="N35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36" t="s">
+        <v>110</v>
+      </c>
+      <c r="K36" t="s">
+        <v>122</v>
+      </c>
+      <c r="L36" t="s">
+        <v>138</v>
+      </c>
+      <c r="M36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H37" t="s">
+        <v>89</v>
+      </c>
+      <c r="I37" t="s">
+        <v>98</v>
+      </c>
+      <c r="J37" t="s">
+        <v>108</v>
+      </c>
+      <c r="K37" t="s">
+        <v>123</v>
+      </c>
+      <c r="L37" t="s">
+        <v>130</v>
+      </c>
+      <c r="M37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" t="s">
+        <v>90</v>
+      </c>
+      <c r="I38" t="s">
+        <v>96</v>
+      </c>
+      <c r="J38" t="s">
+        <v>106</v>
+      </c>
+      <c r="K38" t="s">
+        <v>124</v>
+      </c>
+      <c r="L38" t="s">
+        <v>136</v>
+      </c>
+      <c r="M38" t="s">
+        <v>141</v>
+      </c>
+      <c r="N38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H39" t="s">
+        <v>91</v>
+      </c>
+      <c r="I39" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" t="s">
+        <v>107</v>
+      </c>
+      <c r="K39" t="s">
+        <v>125</v>
+      </c>
+      <c r="L39" t="s">
+        <v>137</v>
+      </c>
+      <c r="M39" t="s">
+        <v>141</v>
+      </c>
+      <c r="N39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" t="s">
+        <v>75</v>
+      </c>
+      <c r="H40" t="s">
+        <v>92</v>
+      </c>
+      <c r="I40" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K40" t="s">
+        <v>126</v>
+      </c>
+      <c r="N40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" t="s">
+        <v>92</v>
+      </c>
+      <c r="I41" t="s">
+        <v>98</v>
+      </c>
+      <c r="J41" t="s">
+        <v>106</v>
+      </c>
+      <c r="K41" t="s">
+        <v>127</v>
+      </c>
+      <c r="L41" t="s">
+        <v>139</v>
+      </c>
+      <c r="M41" t="s">
+        <v>143</v>
+      </c>
+      <c r="N41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" t="s">
+        <v>111</v>
+      </c>
+      <c r="K43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" t="s">
+        <v>39</v>
+      </c>
+      <c r="F46" t="s">
+        <v>41</v>
+      </c>
+      <c r="G46" t="s">
+        <v>59</v>
+      </c>
+      <c r="H46" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" t="s">
+        <v>93</v>
+      </c>
+      <c r="J46" t="s">
+        <v>103</v>
+      </c>
+      <c r="K46" t="s">
+        <v>112</v>
+      </c>
+      <c r="L46" t="s">
+        <v>129</v>
+      </c>
+      <c r="M46" t="s">
+        <v>141</v>
+      </c>
+      <c r="N46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
+        <v>39</v>
+      </c>
+      <c r="F47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" t="s">
+        <v>77</v>
+      </c>
+      <c r="I47" t="s">
+        <v>94</v>
+      </c>
+      <c r="J47" t="s">
+        <v>104</v>
+      </c>
+      <c r="K47" t="s">
+        <v>113</v>
+      </c>
+      <c r="L47" t="s">
+        <v>130</v>
+      </c>
+      <c r="M47" t="s">
+        <v>141</v>
+      </c>
+      <c r="N47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" t="s">
+        <v>39</v>
+      </c>
+      <c r="F48" t="s">
+        <v>43</v>
+      </c>
+      <c r="G48" t="s">
+        <v>61</v>
+      </c>
+      <c r="H48" t="s">
+        <v>78</v>
+      </c>
+      <c r="I48" t="s">
+        <v>95</v>
+      </c>
+      <c r="J48" t="s">
+        <v>105</v>
+      </c>
+      <c r="K48" t="s">
+        <v>114</v>
+      </c>
+      <c r="L48" t="s">
+        <v>131</v>
+      </c>
+      <c r="M48" t="s">
+        <v>141</v>
+      </c>
+      <c r="N48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" t="s">
+        <v>62</v>
+      </c>
+      <c r="H49" t="s">
+        <v>79</v>
+      </c>
+      <c r="I49" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" t="s">
+        <v>115</v>
+      </c>
+      <c r="L49" t="s">
+        <v>132</v>
+      </c>
+      <c r="M49" t="s">
+        <v>141</v>
+      </c>
+      <c r="N49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" t="s">
+        <v>39</v>
+      </c>
+      <c r="F50" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" t="s">
+        <v>97</v>
+      </c>
+      <c r="J50" t="s">
+        <v>107</v>
+      </c>
+      <c r="K50" t="s">
+        <v>116</v>
+      </c>
+      <c r="L50" t="s">
+        <v>133</v>
+      </c>
+      <c r="M50" t="s">
+        <v>141</v>
+      </c>
+      <c r="N50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" t="s">
+        <v>39</v>
+      </c>
+      <c r="F51" t="s">
+        <v>46</v>
+      </c>
+      <c r="G51" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" t="s">
+        <v>81</v>
+      </c>
+      <c r="I51" t="s">
+        <v>97</v>
+      </c>
+      <c r="J51" t="s">
+        <v>107</v>
+      </c>
+      <c r="K51" t="s">
+        <v>117</v>
+      </c>
+      <c r="L51" t="s">
+        <v>134</v>
+      </c>
+      <c r="M51" t="s">
+        <v>142</v>
+      </c>
+      <c r="N51" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" t="s">
+        <v>65</v>
+      </c>
+      <c r="H52" t="s">
+        <v>82</v>
+      </c>
+      <c r="I52" t="s">
+        <v>98</v>
+      </c>
+      <c r="J52" t="s">
+        <v>108</v>
+      </c>
+      <c r="K52" t="s">
+        <v>118</v>
+      </c>
+      <c r="L52" t="s">
+        <v>135</v>
+      </c>
+      <c r="M52" t="s">
+        <v>143</v>
+      </c>
+      <c r="N52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" t="s">
+        <v>48</v>
+      </c>
+      <c r="G53" t="s">
+        <v>66</v>
+      </c>
+      <c r="H53" t="s">
+        <v>83</v>
+      </c>
+      <c r="I53" t="s">
+        <v>99</v>
+      </c>
+      <c r="J53" t="s">
+        <v>109</v>
+      </c>
+      <c r="K53" t="s">
+        <v>119</v>
+      </c>
+      <c r="L53" t="s">
+        <v>136</v>
+      </c>
+      <c r="M53" t="s">
+        <v>143</v>
+      </c>
+      <c r="N53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" t="s">
+        <v>67</v>
+      </c>
+      <c r="H54" t="s">
+        <v>84</v>
+      </c>
+      <c r="I54" t="s">
+        <v>100</v>
+      </c>
+      <c r="J54" t="s">
+        <v>107</v>
+      </c>
+      <c r="K54" t="s">
+        <v>120</v>
+      </c>
+      <c r="L54" t="s">
+        <v>137</v>
+      </c>
+      <c r="M54" t="s">
+        <v>143</v>
+      </c>
+      <c r="N54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" t="s">
+        <v>39</v>
+      </c>
+      <c r="F55" t="s">
+        <v>50</v>
+      </c>
+      <c r="G55" t="s">
+        <v>68</v>
+      </c>
+      <c r="H55" t="s">
+        <v>85</v>
+      </c>
+      <c r="I55" t="s">
+        <v>101</v>
+      </c>
+      <c r="J55" t="s">
+        <v>110</v>
+      </c>
+      <c r="K55" t="s">
+        <v>121</v>
+      </c>
+      <c r="L55" t="s">
+        <v>134</v>
+      </c>
+      <c r="M55" t="s">
+        <v>141</v>
+      </c>
+      <c r="N55" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" t="s">
+        <v>51</v>
+      </c>
+      <c r="G56" t="s">
+        <v>69</v>
+      </c>
+      <c r="H56" t="s">
+        <v>86</v>
+      </c>
+      <c r="I56" t="s">
+        <v>96</v>
+      </c>
+      <c r="J56" t="s">
+        <v>106</v>
+      </c>
+      <c r="K56" t="s">
+        <v>114</v>
+      </c>
+      <c r="L56" t="s">
+        <v>131</v>
+      </c>
+      <c r="M56" t="s">
+        <v>141</v>
+      </c>
+      <c r="N56" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" t="s">
+        <v>39</v>
+      </c>
+      <c r="F57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H57" t="s">
+        <v>87</v>
+      </c>
+      <c r="I57" t="s">
+        <v>96</v>
+      </c>
+      <c r="J57" t="s">
+        <v>106</v>
+      </c>
+      <c r="K57" t="s">
+        <v>121</v>
+      </c>
+      <c r="L57" t="s">
+        <v>134</v>
+      </c>
+      <c r="M57" t="s">
+        <v>141</v>
+      </c>
+      <c r="N57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" t="s">
+        <v>39</v>
+      </c>
+      <c r="F58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G58" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" t="s">
+        <v>88</v>
+      </c>
+      <c r="I58" t="s">
+        <v>101</v>
+      </c>
+      <c r="J58" t="s">
+        <v>110</v>
+      </c>
+      <c r="K58" t="s">
+        <v>122</v>
+      </c>
+      <c r="L58" t="s">
+        <v>138</v>
+      </c>
+      <c r="M58" t="s">
+        <v>141</v>
+      </c>
+      <c r="N58" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" t="s">
+        <v>39</v>
+      </c>
+      <c r="F59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G59" t="s">
+        <v>72</v>
+      </c>
+      <c r="H59" t="s">
+        <v>89</v>
+      </c>
+      <c r="I59" t="s">
+        <v>98</v>
+      </c>
+      <c r="J59" t="s">
+        <v>108</v>
+      </c>
+      <c r="K59" t="s">
+        <v>123</v>
+      </c>
+      <c r="L59" t="s">
+        <v>130</v>
+      </c>
+      <c r="M59" t="s">
+        <v>142</v>
+      </c>
+      <c r="N59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" t="s">
+        <v>39</v>
+      </c>
+      <c r="F60" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60" t="s">
+        <v>73</v>
+      </c>
+      <c r="H60" t="s">
+        <v>90</v>
+      </c>
+      <c r="I60" t="s">
+        <v>96</v>
+      </c>
+      <c r="J60" t="s">
+        <v>106</v>
+      </c>
+      <c r="K60" t="s">
+        <v>124</v>
+      </c>
+      <c r="L60" t="s">
+        <v>136</v>
+      </c>
+      <c r="M60" t="s">
+        <v>141</v>
+      </c>
+      <c r="N60" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" t="s">
+        <v>39</v>
+      </c>
+      <c r="F61" t="s">
+        <v>56</v>
+      </c>
+      <c r="G61" t="s">
+        <v>74</v>
+      </c>
+      <c r="H61" t="s">
+        <v>91</v>
+      </c>
+      <c r="I61" t="s">
+        <v>102</v>
+      </c>
+      <c r="J61" t="s">
+        <v>107</v>
+      </c>
+      <c r="K61" t="s">
+        <v>125</v>
+      </c>
+      <c r="L61" t="s">
+        <v>137</v>
+      </c>
+      <c r="M61" t="s">
+        <v>141</v>
+      </c>
+      <c r="N61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>37</v>
+      </c>
+      <c r="E62" t="s">
+        <v>39</v>
+      </c>
+      <c r="F62" t="s">
+        <v>57</v>
+      </c>
+      <c r="G62" t="s">
+        <v>75</v>
+      </c>
+      <c r="H62" t="s">
+        <v>92</v>
+      </c>
+      <c r="I62" t="s">
+        <v>98</v>
+      </c>
+      <c r="J62" t="s">
+        <v>106</v>
+      </c>
+      <c r="K62" t="s">
+        <v>126</v>
+      </c>
+      <c r="L62" t="s">
+        <v>140</v>
+      </c>
+      <c r="M62" t="s">
+        <v>140</v>
+      </c>
+      <c r="N62" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+      <c r="G63" t="s">
+        <v>75</v>
+      </c>
+      <c r="H63" t="s">
+        <v>92</v>
+      </c>
+      <c r="I63" t="s">
+        <v>98</v>
+      </c>
+      <c r="J63" t="s">
+        <v>106</v>
+      </c>
+      <c r="K63" t="s">
+        <v>127</v>
+      </c>
+      <c r="L63" t="s">
+        <v>139</v>
+      </c>
+      <c r="M63" t="s">
+        <v>143</v>
+      </c>
+      <c r="N63" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="C65" t="s">
+        <v>20</v>
+      </c>
+      <c r="J65" t="s">
+        <v>111</v>
+      </c>
+      <c r="K65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>